<commit_message>
final cleanup and check
</commit_message>
<xml_diff>
--- a/SFUSat-Radio-BoM.xlsx
+++ b/SFUSat-Radio-BoM.xlsx
@@ -14,14 +14,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="840">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -794,7 +794,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">D3, </t>
     </r>
@@ -802,9 +801,8 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">D11, D1, D420, D421, D2, D4</t>
     </r>
@@ -1653,7 +1651,7 @@
     <t xml:space="preserve">2.37 MOhms</t>
   </si>
   <si>
-    <t xml:space="preserve">L4, L</t>
+    <t xml:space="preserve">L4</t>
   </si>
   <si>
     <t xml:space="preserve">10uH</t>
@@ -1702,6 +1700,36 @@
   </si>
   <si>
     <t xml:space="preserve">1.6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFUSat-ind:SLF7045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLF7045T-100M1R3-PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonstandard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.276" L x 0.276" W (7.00mm x 7.00mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-2014-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.78A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43.2 mOhm Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3A</t>
   </si>
   <si>
     <t xml:space="preserve">C36</t>
@@ -2565,14 +2593,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2617,7 +2643,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2631,6 +2657,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2653,8 +2683,8 @@
   </sheetPr>
   <dimension ref="A1:ED267"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A217" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B237" activeCellId="1" sqref="G1:G25 B237"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A245" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4132,11 +4162,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4146,10 +4176,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:EB83"/>
+  <dimension ref="A1:EB84"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1:G25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H45" activeCellId="0" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6191,7 +6221,7 @@
         <v>541</v>
       </c>
       <c r="H43" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>383</v>
@@ -6260,471 +6290,477 @@
         <v>553</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+    <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="H44" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="P44" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="Q44" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="H44" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="T44" s="1" t="s">
+      <c r="S44" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="T44" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="W44" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="X44" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="Y44" s="1" t="s">
+      <c r="W44" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="X44" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y44" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AB44" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="AC44" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="AK44" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="AS44" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="AV44" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="AW44" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="AX44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AY44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AZ44" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BA44" s="1" t="s">
+      <c r="Z44" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA44" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="BB44" s="1" t="s">
-        <v>513</v>
+      <c r="AC44" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="AK44" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="AS44" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="AT44" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="AZ44" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="BC44" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="BD44" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="BF44" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="BG44" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="BH44" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="BI44" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="BJ44" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="DK44" s="4" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>562</v>
+        <v>312</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="H45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>565</v>
+        <v>271</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>356</v>
+        <v>273</v>
       </c>
       <c r="T45" s="1" t="s">
         <v>167</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>566</v>
+        <v>377</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>522</v>
       </c>
       <c r="Y45" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="Z45" s="1" t="s">
-        <v>567</v>
+      <c r="AB45" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="AC45" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="AK45" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="AN45" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AS45" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AV45" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AW45" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="AS45" s="1" t="s">
+      <c r="AX45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AY45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA45" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="BB45" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="Y46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="AK46" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="AN46" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="AS46" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="DL45" s="1" t="s">
+      <c r="DL46" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="DM45" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="DN45" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="DO45" s="1" t="n">
+      <c r="DM46" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="DN46" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="DO46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="DP45" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="DQ45" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="DR45" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="DS45" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="DT45" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="DU45" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="DV45" s="1" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="DP46" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="DQ46" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="DR46" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="DS46" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="DT46" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="DU46" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="DV46" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="H46" s="1" t="n">
+      <c r="D47" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="H47" s="1" t="n">
         <v>5</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="H47" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>145</v>
+        <v>596</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>597</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>209</v>
+        <v>598</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>210</v>
+        <v>599</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>595</v>
+        <v>145</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>596</v>
+        <v>209</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>597</v>
+        <v>210</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>602</v>
+        <v>606</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>607</v>
       </c>
       <c r="H50" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
-        <v>603</v>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>608</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="H51" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="H51" s="1" t="n">
+      <c r="D52" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="H52" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="L51" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="S51" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="T51" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="W51" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="X51" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="Y51" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB51" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="AC51" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="AK51" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="AS51" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="AV51" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="AW51" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="AX51" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AY51" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AZ51" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BA51" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="BB51" s="1" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="H52" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="L52" s="1" t="s">
-        <v>378</v>
+        <v>159</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>616</v>
+        <v>159</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O52" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="S52" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>618</v>
       </c>
       <c r="T52" s="1" t="s">
         <v>167</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>619</v>
+        <v>377</v>
       </c>
       <c r="X52" s="1" t="s">
-        <v>620</v>
+        <v>508</v>
       </c>
       <c r="Y52" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="AB52" s="1" t="s">
+        <v>509</v>
+      </c>
       <c r="AC52" s="1" t="s">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="AK52" s="1" t="s">
-        <v>277</v>
+        <v>510</v>
       </c>
       <c r="AS52" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="AT52" s="1" t="s">
-        <v>621</v>
+        <v>278</v>
+      </c>
+      <c r="AV52" s="1" t="s">
+        <v>378</v>
       </c>
       <c r="AW52" s="1" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="AX52" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="AY52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA52" s="1" t="s">
+        <v>512</v>
+      </c>
       <c r="BB52" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="BQ52" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="BR52" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BS52" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>625</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="H53" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>615</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>159</v>
@@ -6733,34 +6769,34 @@
         <v>378</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="T53" s="1" t="s">
         <v>167</v>
       </c>
       <c r="W53" s="1" t="s">
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="X53" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="Y53" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AC53" s="1" t="s">
-        <v>440</v>
+        <v>568</v>
       </c>
       <c r="AK53" s="1" t="s">
         <v>277</v>
@@ -6769,16 +6805,16 @@
         <v>362</v>
       </c>
       <c r="AT53" s="1" t="s">
-        <v>621</v>
+        <v>631</v>
       </c>
       <c r="AW53" s="1" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="AX53" s="1" t="s">
         <v>159</v>
       </c>
       <c r="BB53" s="1" t="s">
-        <v>632</v>
+        <v>444</v>
       </c>
       <c r="BQ53" s="1" t="s">
         <v>633</v>
@@ -6790,12 +6826,12 @@
         <v>634</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>635</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>636</v>
@@ -6807,22 +6843,25 @@
         <v>638</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>271</v>
+        <v>625</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>159</v>
+        <v>378</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>159</v>
+        <v>639</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="P54" s="1" t="s">
         <v>637</v>
@@ -6834,66 +6873,63 @@
         <v>167</v>
       </c>
       <c r="W54" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="X54" s="1" t="s">
         <v>641</v>
-      </c>
-      <c r="X54" s="1" t="s">
-        <v>642</v>
       </c>
       <c r="Y54" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AB54" s="1" t="s">
-        <v>509</v>
-      </c>
       <c r="AC54" s="1" t="s">
-        <v>558</v>
+        <v>440</v>
       </c>
       <c r="AK54" s="1" t="s">
-        <v>510</v>
+        <v>277</v>
       </c>
       <c r="AS54" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="AV54" s="1" t="s">
-        <v>378</v>
+        <v>362</v>
+      </c>
+      <c r="AT54" s="1" t="s">
+        <v>631</v>
       </c>
       <c r="AW54" s="1" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="AX54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="AY54" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AZ54" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BA54" s="1" t="s">
-        <v>616</v>
-      </c>
       <c r="BB54" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="BQ54" s="1" t="s">
         <v>643</v>
       </c>
+      <c r="BR54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BS54" s="1" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>645</v>
+      </c>
       <c r="B55" s="1" t="s">
-        <v>644</v>
+        <v>621</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>240</v>
+        <v>646</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="H55" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>271</v>
@@ -6908,22 +6944,22 @@
         <v>162</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>273</v>
+        <v>649</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>166</v>
+        <v>650</v>
       </c>
       <c r="T55" s="1" t="s">
         <v>167</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>377</v>
+        <v>651</v>
       </c>
       <c r="X55" s="1" t="s">
-        <v>171</v>
+        <v>652</v>
       </c>
       <c r="Y55" s="1" t="s">
         <v>172</v>
@@ -6932,7 +6968,7 @@
         <v>509</v>
       </c>
       <c r="AC55" s="1" t="s">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="AK55" s="1" t="s">
         <v>510</v>
@@ -6944,16 +6980,19 @@
         <v>378</v>
       </c>
       <c r="AW55" s="1" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="AX55" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="AY55" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="AZ55" s="1" t="s">
         <v>159</v>
       </c>
       <c r="BA55" s="1" t="s">
-        <v>280</v>
+        <v>626</v>
       </c>
       <c r="BB55" s="1" t="s">
         <v>444</v>
@@ -6961,99 +7000,102 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
       <c r="H56" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>159</v>
+        <v>271</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>518</v>
+        <v>159</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>163</v>
+        <v>273</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="R56" s="1" t="n">
-        <v>2</v>
+        <v>655</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>652</v>
+        <v>166</v>
       </c>
       <c r="T56" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="U56" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="V56" s="1" t="s">
-        <v>653</v>
-      </c>
       <c r="W56" s="1" t="s">
-        <v>521</v>
+        <v>377</v>
       </c>
       <c r="X56" s="1" t="s">
-        <v>522</v>
+        <v>171</v>
       </c>
       <c r="Y56" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="Z56" s="1" t="n">
-        <v>805</v>
-      </c>
       <c r="AB56" s="1" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="AC56" s="1" t="s">
-        <v>524</v>
+        <v>568</v>
       </c>
       <c r="AK56" s="1" t="s">
-        <v>176</v>
+        <v>510</v>
+      </c>
+      <c r="AS56" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AV56" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AW56" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="AX56" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ56" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA56" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="BB56" s="1" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>223</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="H57" s="1" t="n">
         <v>1</v>
@@ -7080,13 +7122,13 @@
         <v>163</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="R57" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="T57" s="1" t="s">
         <v>167</v>
@@ -7095,7 +7137,7 @@
         <v>519</v>
       </c>
       <c r="V57" s="1" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>521</v>
@@ -7121,19 +7163,19 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="H58" s="1" t="n">
         <v>1</v>
@@ -7151,43 +7193,43 @@
         <v>160</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>161</v>
+        <v>518</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>529</v>
+        <v>163</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="R58" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>166</v>
+        <v>662</v>
       </c>
       <c r="T58" s="1" t="s">
         <v>167</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>168</v>
+        <v>519</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="W58" s="1" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="X58" s="1" t="s">
-        <v>171</v>
+        <v>522</v>
       </c>
       <c r="Y58" s="1" t="s">
         <v>172</v>
       </c>
       <c r="Z58" s="1" t="n">
-        <v>402</v>
+        <v>805</v>
       </c>
       <c r="AB58" s="1" t="s">
         <v>523</v>
@@ -7201,105 +7243,99 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>555</v>
+        <v>152</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="H59" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>271</v>
+        <v>157</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>273</v>
+        <v>529</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>666</v>
+        <v>671</v>
+      </c>
+      <c r="R59" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>652</v>
+        <v>166</v>
       </c>
       <c r="T59" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="U59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>673</v>
+      </c>
       <c r="W59" s="1" t="s">
-        <v>377</v>
+        <v>531</v>
       </c>
       <c r="X59" s="1" t="s">
-        <v>522</v>
+        <v>171</v>
       </c>
       <c r="Y59" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="Z59" s="1" t="n">
+        <v>402</v>
+      </c>
       <c r="AB59" s="1" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="AC59" s="1" t="s">
-        <v>558</v>
+        <v>524</v>
       </c>
       <c r="AK59" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="AS59" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="AV59" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="AW59" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="AX59" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AY59" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AZ59" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BA59" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="BB59" s="1" t="s">
-        <v>513</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>240</v>
+        <v>565</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
       <c r="H60" s="1" t="n">
         <v>1</v>
@@ -7320,10 +7356,10 @@
         <v>273</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="S60" s="1" t="s">
-        <v>166</v>
+        <v>662</v>
       </c>
       <c r="T60" s="1" t="s">
         <v>167</v>
@@ -7332,19 +7368,19 @@
         <v>377</v>
       </c>
       <c r="X60" s="1" t="s">
-        <v>171</v>
+        <v>522</v>
       </c>
       <c r="Y60" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AB60" s="1" t="s">
-        <v>275</v>
+        <v>509</v>
       </c>
       <c r="AC60" s="1" t="s">
-        <v>276</v>
+        <v>568</v>
       </c>
       <c r="AK60" s="1" t="s">
-        <v>277</v>
+        <v>510</v>
       </c>
       <c r="AS60" s="1" t="s">
         <v>278</v>
@@ -7353,7 +7389,7 @@
         <v>378</v>
       </c>
       <c r="AW60" s="1" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="AX60" s="1" t="s">
         <v>159</v>
@@ -7365,27 +7401,27 @@
         <v>159</v>
       </c>
       <c r="BA60" s="1" t="s">
-        <v>280</v>
+        <v>384</v>
       </c>
       <c r="BB60" s="1" t="s">
-        <v>632</v>
+        <v>513</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>674</v>
+        <v>680</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>240</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="H61" s="1" t="n">
         <v>1</v>
@@ -7406,7 +7442,7 @@
         <v>273</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="S61" s="1" t="s">
         <v>166</v>
@@ -7424,13 +7460,13 @@
         <v>172</v>
       </c>
       <c r="AB61" s="1" t="s">
-        <v>509</v>
+        <v>275</v>
       </c>
       <c r="AC61" s="1" t="s">
-        <v>558</v>
+        <v>276</v>
       </c>
       <c r="AK61" s="1" t="s">
-        <v>510</v>
+        <v>277</v>
       </c>
       <c r="AS61" s="1" t="s">
         <v>278</v>
@@ -7439,7 +7475,7 @@
         <v>378</v>
       </c>
       <c r="AW61" s="1" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="AX61" s="1" t="s">
         <v>159</v>
@@ -7454,593 +7490,656 @@
         <v>280</v>
       </c>
       <c r="BB61" s="1" t="s">
-        <v>609</v>
+        <v>642</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>679</v>
+        <v>684</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>680</v>
+        <v>240</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="H62" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="T62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="W62" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="X62" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y62" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB62" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="AC62" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="AK62" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="AS62" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AV62" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="AW62" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="AX62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AY62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ62" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA62" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="BB62" s="1" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>684</v>
+        <v>689</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>686</v>
-      </c>
-      <c r="E63" s="2" t="str">
+        <v>690</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="E64" s="2" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.ca/products/en?keywords=2N7002DW-FDICT-ND","2N7002DW-FDICT-ND")</f>
         <v>2N7002DW-FDICT-ND</v>
       </c>
-      <c r="H63" s="1" t="n">
+      <c r="H64" s="1" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="H64" s="1" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>265</v>
+        <v>145</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>286</v>
+        <v>700</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="H65" s="1" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>696</v>
+    <row r="66" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>702</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>698</v>
+        <v>265</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>700</v>
+        <v>286</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>705</v>
+        <v>710</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>711</v>
       </c>
       <c r="H67" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="N67" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O67" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="T67" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="U67" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="V67" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="W67" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="X67" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="Y67" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB67" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="AC67" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="AS67" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="BX67" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="BY67" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ67" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="CA67" s="1" t="s">
-        <v>715</v>
-      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>240</v>
+        <v>714</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="H68" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="L68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>159</v>
+        <v>716</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="S68" s="1" t="s">
-        <v>166</v>
+        <v>717</v>
       </c>
       <c r="T68" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="U68" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="V68" s="1" t="s">
+        <v>719</v>
+      </c>
       <c r="W68" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="X68" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="X68" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="Y68" s="1" t="s">
         <v>172</v>
       </c>
       <c r="AB68" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AC68" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="AS68" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="BX68" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="BY68" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ68" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="CA68" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="H69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O69" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="S69" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="T69" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="W69" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="X69" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y69" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB69" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="AC68" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="AK68" s="1" t="s">
+      <c r="AC69" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="AK69" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="AS68" s="1" t="s">
+      <c r="AS69" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="AV68" s="1" t="s">
+      <c r="AV69" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="AW68" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="AX68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AY68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="AZ68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BA68" s="1" t="s">
+      <c r="AW69" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="AX69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AY69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AZ69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA69" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="BB68" s="1" t="s">
+      <c r="BB69" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
-        <v>723</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C69" s="1" t="s">
+    <row r="70" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>725</v>
-      </c>
-      <c r="E69" s="2" t="str">
+      <c r="D70" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="E70" s="2" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.ca/products/en?keywords=490-5942-1-ND","490-5942-1-ND")</f>
         <v>490-5942-1-ND</v>
       </c>
-      <c r="H69" s="1" t="n">
+      <c r="H70" s="1" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="C70" s="1" t="s">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="E70" s="2" t="str">
+      <c r="D71" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="E71" s="2" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.ca/products/en?keywords=P56.0KLCT-ND","P56.0KLCT-ND")</f>
         <v>P56.0KLCT-ND</v>
       </c>
-      <c r="H70" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>733</v>
-      </c>
       <c r="H71" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="CI71" s="1" t="s">
-        <v>734</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="H72" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="CI72" s="1" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>744</v>
+        <v>749</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>750</v>
       </c>
       <c r="H73" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="L73" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="N73" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O73" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="S73" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="T73" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="W73" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="Y73" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z73" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="AK73" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="AO73" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="AP73" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="AQ73" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="AS73" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="CB73" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="CC73" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="CD73" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="CE73" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="CF73" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="CG73" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="CH73" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="H74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="S74" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="T74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="W74" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="Y74" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z74" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="AK74" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="AO74" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="AP74" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="AQ74" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="AS74" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CB74" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="CC74" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="CD74" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="CE74" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="CF74" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="CG74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH74" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="E74" s="2" t="str">
+      <c r="D75" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="E75" s="2" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.ca/products/en?keywords=490-3254-1-ND","490-3254-1-ND")</f>
         <v>490-3254-1-ND</v>
       </c>
-      <c r="H74" s="1" t="n">
+      <c r="H75" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>763</v>
-      </c>
-      <c r="E75" s="2" t="str">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="E76" s="2" t="str">
         <f aca="false">HYPERLINK("http://www.digikey.ca/products/en?keywords=863-1645-1-ND","863-1645-1-ND")</f>
         <v>863-1645-1-ND</v>
       </c>
-      <c r="H75" s="1" t="n">
+      <c r="H76" s="1" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="H76" s="1" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>769</v>
+        <v>415</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>265</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>771</v>
+        <v>286</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="H77" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="H78" s="1" t="n">
         <v>8</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="H78" s="1" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>416</v>
+        <v>786</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>417</v>
+        <v>787</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>782</v>
+        <v>788</v>
       </c>
       <c r="H79" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="B80" s="1" t="n">
-        <v>100</v>
+        <v>789</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>790</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>265</v>
+        <v>791</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>784</v>
+        <v>416</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>785</v>
+        <v>417</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c r="H80" s="1" t="n">
         <v>1</v>
@@ -8048,19 +8147,22 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>788</v>
+        <v>793</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>789</v>
+        <v>265</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>791</v>
+        <v>795</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>796</v>
       </c>
       <c r="H81" s="1" t="n">
         <v>1</v>
@@ -8068,201 +8170,221 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>792</v>
+        <v>797</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>794</v>
+        <v>799</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>793</v>
+        <v>800</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>795</v>
+        <v>801</v>
       </c>
       <c r="H82" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="N82" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O82" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="T82" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="W82" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="Y82" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AS82" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="AT82" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="BT82" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="BU82" s="1" t="s">
-        <v>801</v>
-      </c>
-      <c r="BV82" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BW82" s="1" t="s">
-        <v>802</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>807</v>
       </c>
       <c r="H83" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>162</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="T83" s="1" t="s">
         <v>167</v>
       </c>
       <c r="W83" s="1" t="s">
-        <v>811</v>
+        <v>159</v>
       </c>
       <c r="Y83" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="AK83" s="1" t="s">
+      <c r="AS83" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="AT83" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="BT83" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="BU83" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="BV83" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BW83" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="H84" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="N84" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="T84" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="W84" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="Y84" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK84" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="AS83" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="AV83" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="BC83" s="1" t="s">
-        <v>812</v>
-      </c>
-      <c r="CJ83" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="CK83" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="CL83" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="CM83" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="CN83" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="CO83" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="CP83" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="CQ83" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="CR83" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="CS83" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="CT83" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="CU83" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="CV83" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="CW83" s="1" t="s">
+      <c r="AS84" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="AV84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BC84" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="CX83" s="1" t="s">
+      <c r="CJ84" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="CY83" s="1" t="s">
+      <c r="CK84" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="CZ83" s="1" t="s">
+      <c r="CL84" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="CM84" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="DA83" s="1" t="n">
+      <c r="CN84" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="CO84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="CP84" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="CQ84" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="CR84" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="CS84" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="CT84" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="CU84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="CV84" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="CW84" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="CX84" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="CY84" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="CZ84" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="DA84" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="DB83" s="1" t="s">
-        <v>826</v>
-      </c>
-      <c r="DC83" s="1" t="n">
+      <c r="DB84" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="DC84" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="DD83" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="DE83" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="DF83" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="DG83" s="1" t="s">
-        <v>828</v>
-      </c>
-      <c r="DH83" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="DI83" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="DJ83" s="1" t="s">
+      <c r="DD84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="DE84" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="DF84" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="DG84" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="DH84" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="DI84" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="DJ84" s="1" t="s">
         <v>159</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>